<commit_message>
Updated progress of batch 1
</commit_message>
<xml_diff>
--- a/spring-boot/Teams Progress/batch1-2025-teams.xlsx
+++ b/spring-boot/Teams Progress/batch1-2025-teams.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Training-Teaching\bv-raju\training-materials\Teams Progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Training-Teaching\bv-raju\training-materials\spring-boot\Teams Progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36583D1-D07E-4000-AC53-6B4B0BA42AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3359D4-EB89-4922-9CCB-1490005C1861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1507,7 +1507,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1522,6 +1522,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1553,7 +1565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1561,6 +1573,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1875,10 +1889,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1915,7 +1930,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1931,10 +1946,10 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1950,10 +1965,10 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1969,10 +1984,10 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1988,10 +2003,10 @@
       <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -2007,10 +2022,10 @@
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2026,10 +2041,10 @@
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2045,10 +2060,10 @@
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -2064,10 +2079,10 @@
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -2083,10 +2098,10 @@
       <c r="E10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -2102,10 +2117,10 @@
       <c r="E11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -2121,10 +2136,10 @@
       <c r="E12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -2140,10 +2155,10 @@
       <c r="E13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
@@ -2159,10 +2174,10 @@
       <c r="E14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
@@ -2178,10 +2193,10 @@
       <c r="E15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
@@ -2197,10 +2212,10 @@
       <c r="E16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -2216,10 +2231,10 @@
       <c r="E17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
@@ -2235,10 +2250,10 @@
       <c r="E18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>60</v>
       </c>
@@ -2254,10 +2269,10 @@
       <c r="E19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -2276,7 +2291,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>67</v>
       </c>
@@ -2292,10 +2307,10 @@
       <c r="E21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>70</v>
       </c>
@@ -2314,7 +2329,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>73</v>
       </c>
@@ -2333,7 +2348,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>76</v>
       </c>
@@ -2352,7 +2367,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>79</v>
       </c>
@@ -2371,7 +2386,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>82</v>
       </c>
@@ -2387,10 +2402,10 @@
       <c r="E26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>85</v>
       </c>
@@ -2409,7 +2424,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>88</v>
       </c>
@@ -2428,7 +2443,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>91</v>
       </c>
@@ -2447,7 +2462,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>94</v>
       </c>
@@ -2463,10 +2478,10 @@
       <c r="E30" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="5"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>98</v>
       </c>
@@ -2482,10 +2497,10 @@
       <c r="E31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="5"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>101</v>
       </c>
@@ -2501,10 +2516,10 @@
       <c r="E32" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>104</v>
       </c>
@@ -2520,10 +2535,10 @@
       <c r="E33" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F33" s="2"/>
+      <c r="F33" s="5"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>107</v>
       </c>
@@ -2539,10 +2554,10 @@
       <c r="E34" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>110</v>
       </c>
@@ -2558,10 +2573,10 @@
       <c r="E35" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F35" s="2"/>
+      <c r="F35" s="5"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>113</v>
       </c>
@@ -2577,10 +2592,10 @@
       <c r="E36" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>116</v>
       </c>
@@ -2596,10 +2611,10 @@
       <c r="E37" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>119</v>
       </c>
@@ -2615,10 +2630,10 @@
       <c r="E38" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="2"/>
+      <c r="F38" s="5"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>122</v>
       </c>
@@ -2634,10 +2649,10 @@
       <c r="E39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F39" s="2"/>
+      <c r="F39" s="5"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>125</v>
       </c>
@@ -2653,10 +2668,10 @@
       <c r="E40" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="5"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>129</v>
       </c>
@@ -2672,10 +2687,10 @@
       <c r="E41" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F41" s="2"/>
+      <c r="F41" s="5"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>132</v>
       </c>
@@ -2691,10 +2706,10 @@
       <c r="E42" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="F42" s="2"/>
+      <c r="F42" s="5"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>135</v>
       </c>
@@ -2710,10 +2725,10 @@
       <c r="E43" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F43" s="2"/>
+      <c r="F43" s="5"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>138</v>
       </c>
@@ -2729,10 +2744,10 @@
       <c r="E44" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F44" s="2"/>
+      <c r="F44" s="5"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>141</v>
       </c>
@@ -2748,10 +2763,10 @@
       <c r="E45" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F45" s="2"/>
+      <c r="F45" s="5"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>144</v>
       </c>
@@ -2767,10 +2782,10 @@
       <c r="E46" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F46" s="2"/>
+      <c r="F46" s="5"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>147</v>
       </c>
@@ -2786,10 +2801,10 @@
       <c r="E47" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F47" s="2"/>
+      <c r="F47" s="5"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>150</v>
       </c>
@@ -2805,10 +2820,10 @@
       <c r="E48" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F48" s="2"/>
+      <c r="F48" s="5"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>153</v>
       </c>
@@ -2824,10 +2839,10 @@
       <c r="E49" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F49" s="2"/>
+      <c r="F49" s="5"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>156</v>
       </c>
@@ -2843,10 +2858,10 @@
       <c r="E50" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F50" s="2"/>
+      <c r="F50" s="5"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>160</v>
       </c>
@@ -2862,10 +2877,10 @@
       <c r="E51" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F51" s="2"/>
+      <c r="F51" s="5"/>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
         <v>486</v>
@@ -2879,10 +2894,10 @@
       <c r="E52" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F52" s="2"/>
+      <c r="F52" s="5"/>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>163</v>
       </c>
@@ -2898,10 +2913,10 @@
       <c r="E53" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F53" s="2"/>
+      <c r="F53" s="5"/>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>168</v>
       </c>
@@ -2917,10 +2932,10 @@
       <c r="E54" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F54" s="2"/>
+      <c r="F54" s="5"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>171</v>
       </c>
@@ -2936,10 +2951,10 @@
       <c r="E55" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F55" s="2"/>
+      <c r="F55" s="5"/>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>174</v>
       </c>
@@ -2955,10 +2970,10 @@
       <c r="E56" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F56" s="2"/>
+      <c r="F56" s="5"/>
       <c r="G56" s="2"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>177</v>
       </c>
@@ -2974,10 +2989,10 @@
       <c r="E57" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F57" s="2"/>
+      <c r="F57" s="5"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>180</v>
       </c>
@@ -2993,10 +3008,10 @@
       <c r="E58" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F58" s="2"/>
+      <c r="F58" s="5"/>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>183</v>
       </c>
@@ -3012,10 +3027,10 @@
       <c r="E59" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F59" s="2"/>
+      <c r="F59" s="5"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>186</v>
       </c>
@@ -3031,10 +3046,10 @@
       <c r="E60" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F60" s="2"/>
+      <c r="F60" s="5"/>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>189</v>
       </c>
@@ -3050,10 +3065,10 @@
       <c r="E61" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F61" s="2"/>
+      <c r="F61" s="5"/>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>192</v>
       </c>
@@ -3069,10 +3084,10 @@
       <c r="E62" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F62" s="2"/>
+      <c r="F62" s="5"/>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>195</v>
       </c>
@@ -3088,10 +3103,10 @@
       <c r="E63" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F63" s="2"/>
+      <c r="F63" s="5"/>
       <c r="G63" s="2"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>199</v>
       </c>
@@ -3107,10 +3122,10 @@
       <c r="E64" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F64" s="2"/>
+      <c r="F64" s="5"/>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>202</v>
       </c>
@@ -3126,10 +3141,10 @@
       <c r="E65" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F65" s="2"/>
+      <c r="F65" s="5"/>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>205</v>
       </c>
@@ -3145,10 +3160,10 @@
       <c r="E66" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F66" s="2"/>
+      <c r="F66" s="5"/>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>208</v>
       </c>
@@ -3164,10 +3179,10 @@
       <c r="E67" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F67" s="2"/>
+      <c r="F67" s="6"/>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>211</v>
       </c>
@@ -3183,10 +3198,10 @@
       <c r="E68" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F68" s="2"/>
+      <c r="F68" s="5"/>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>214</v>
       </c>
@@ -3202,10 +3217,10 @@
       <c r="E69" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F69" s="2"/>
+      <c r="F69" s="5"/>
       <c r="G69" s="2"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>217</v>
       </c>
@@ -3221,10 +3236,10 @@
       <c r="E70" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F70" s="2"/>
+      <c r="F70" s="5"/>
       <c r="G70" s="2"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>220</v>
       </c>
@@ -3240,10 +3255,10 @@
       <c r="E71" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F71" s="2"/>
+      <c r="F71" s="5"/>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>223</v>
       </c>
@@ -3259,10 +3274,10 @@
       <c r="E72" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F72" s="2"/>
+      <c r="F72" s="5"/>
       <c r="G72" s="2"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>226</v>
       </c>
@@ -3278,10 +3293,10 @@
       <c r="E73" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="F73" s="2"/>
+      <c r="F73" s="5"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>230</v>
       </c>
@@ -3297,10 +3312,10 @@
       <c r="E74" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="F74" s="2"/>
+      <c r="F74" s="5"/>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>233</v>
       </c>
@@ -3316,10 +3331,10 @@
       <c r="E75" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="F75" s="2"/>
+      <c r="F75" s="5"/>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>236</v>
       </c>
@@ -3335,10 +3350,10 @@
       <c r="E76" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="F76" s="2"/>
+      <c r="F76" s="5"/>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>239</v>
       </c>
@@ -3354,10 +3369,10 @@
       <c r="E77" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="F77" s="2"/>
+      <c r="F77" s="5"/>
       <c r="G77" s="2"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>242</v>
       </c>
@@ -3373,10 +3388,10 @@
       <c r="E78" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F78" s="2"/>
+      <c r="F78" s="5"/>
       <c r="G78" s="2"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>247</v>
       </c>
@@ -3392,10 +3407,10 @@
       <c r="E79" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F79" s="2"/>
+      <c r="F79" s="5"/>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>250</v>
       </c>
@@ -3411,10 +3426,10 @@
       <c r="E80" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F80" s="2"/>
+      <c r="F80" s="5"/>
       <c r="G80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>253</v>
       </c>
@@ -3430,10 +3445,10 @@
       <c r="E81" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F81" s="2"/>
+      <c r="F81" s="5"/>
       <c r="G81" s="2"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>256</v>
       </c>
@@ -3449,10 +3464,10 @@
       <c r="E82" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F82" s="2"/>
+      <c r="F82" s="5"/>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>259</v>
       </c>
@@ -3468,10 +3483,10 @@
       <c r="E83" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F83" s="2"/>
+      <c r="F83" s="5"/>
       <c r="G83" s="2"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>262</v>
       </c>
@@ -3487,10 +3502,10 @@
       <c r="E84" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F84" s="2"/>
+      <c r="F84" s="5"/>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>265</v>
       </c>
@@ -3506,10 +3521,10 @@
       <c r="E85" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F85" s="2"/>
+      <c r="F85" s="5"/>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>268</v>
       </c>
@@ -3525,10 +3540,10 @@
       <c r="E86" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="F86" s="2"/>
+      <c r="F86" s="5"/>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>271</v>
       </c>
@@ -3544,10 +3559,10 @@
       <c r="E87" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F87" s="2"/>
+      <c r="F87" s="5"/>
       <c r="G87" s="2"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>274</v>
       </c>
@@ -3566,7 +3581,7 @@
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>278</v>
       </c>
@@ -3585,7 +3600,7 @@
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>281</v>
       </c>
@@ -3604,7 +3619,7 @@
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>284</v>
       </c>
@@ -3623,7 +3638,7 @@
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>287</v>
       </c>
@@ -3639,10 +3654,10 @@
       <c r="E92" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="F92" s="2"/>
+      <c r="F92" s="6"/>
       <c r="G92" s="2"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>290</v>
       </c>
@@ -3661,7 +3676,7 @@
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>293</v>
       </c>
@@ -3677,10 +3692,10 @@
       <c r="E94" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="F94" s="2"/>
+      <c r="F94" s="6"/>
       <c r="G94" s="2"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>296</v>
       </c>
@@ -3699,7 +3714,7 @@
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>299</v>
       </c>
@@ -3718,7 +3733,7 @@
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>302</v>
       </c>
@@ -3737,7 +3752,7 @@
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>305</v>
       </c>
@@ -3756,7 +3771,7 @@
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>309</v>
       </c>
@@ -3775,7 +3790,7 @@
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>312</v>
       </c>
@@ -3794,7 +3809,7 @@
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>315</v>
       </c>
@@ -3810,10 +3825,10 @@
       <c r="E101" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F101" s="2"/>
+      <c r="F101" s="6"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>318</v>
       </c>
@@ -3832,7 +3847,7 @@
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>321</v>
       </c>
@@ -3851,7 +3866,7 @@
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>324</v>
       </c>
@@ -3870,7 +3885,7 @@
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>327</v>
       </c>
@@ -3886,10 +3901,10 @@
       <c r="E105" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F105" s="2"/>
+      <c r="F105" s="6"/>
       <c r="G105" s="2"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>330</v>
       </c>
@@ -3905,10 +3920,10 @@
       <c r="E106" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F106" s="2"/>
+      <c r="F106" s="6"/>
       <c r="G106" s="2"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>333</v>
       </c>
@@ -4209,7 +4224,7 @@
       <c r="E122" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="F122" s="2"/>
+      <c r="F122" s="6"/>
       <c r="G122" s="2"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -4247,7 +4262,7 @@
       <c r="E124" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="F124" s="2"/>
+      <c r="F124" s="6"/>
       <c r="G124" s="2"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -4304,7 +4319,7 @@
       <c r="E127" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="F127" s="2"/>
+      <c r="F127" s="6"/>
       <c r="G127" s="2"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
@@ -4323,7 +4338,7 @@
       <c r="E128" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="F128" s="2"/>
+      <c r="F128" s="6"/>
       <c r="G128" s="2"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -4342,10 +4357,10 @@
       <c r="E129" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="F129" s="2"/>
+      <c r="F129" s="6"/>
       <c r="G129" s="2"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>405</v>
       </c>
@@ -4361,10 +4376,10 @@
       <c r="E130" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F130" s="2"/>
+      <c r="F130" s="5"/>
       <c r="G130" s="2"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>410</v>
       </c>
@@ -4380,10 +4395,10 @@
       <c r="E131" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F131" s="2"/>
+      <c r="F131" s="5"/>
       <c r="G131" s="2"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>413</v>
       </c>
@@ -4399,10 +4414,10 @@
       <c r="E132" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F132" s="2"/>
+      <c r="F132" s="5"/>
       <c r="G132" s="2"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>416</v>
       </c>
@@ -4418,10 +4433,10 @@
       <c r="E133" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F133" s="2"/>
+      <c r="F133" s="5"/>
       <c r="G133" s="2"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>419</v>
       </c>
@@ -4437,10 +4452,10 @@
       <c r="E134" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F134" s="2"/>
+      <c r="F134" s="5"/>
       <c r="G134" s="2"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>422</v>
       </c>
@@ -4456,10 +4471,10 @@
       <c r="E135" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F135" s="2"/>
+      <c r="F135" s="5"/>
       <c r="G135" s="2"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>425</v>
       </c>
@@ -4475,10 +4490,10 @@
       <c r="E136" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F136" s="2"/>
+      <c r="F136" s="5"/>
       <c r="G136" s="2"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>428</v>
       </c>
@@ -4494,10 +4509,10 @@
       <c r="E137" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="F137" s="2"/>
+      <c r="F137" s="5"/>
       <c r="G137" s="2"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>431</v>
       </c>
@@ -4513,10 +4528,10 @@
       <c r="E138" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F138" s="2"/>
+      <c r="F138" s="5"/>
       <c r="G138" s="2"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>434</v>
       </c>
@@ -4532,10 +4547,10 @@
       <c r="E139" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F139" s="2"/>
+      <c r="F139" s="5"/>
       <c r="G139" s="2"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>437</v>
       </c>
@@ -4551,10 +4566,10 @@
       <c r="E140" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F140" s="2"/>
+      <c r="F140" s="5"/>
       <c r="G140" s="2"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>441</v>
       </c>
@@ -4570,10 +4585,10 @@
       <c r="E141" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F141" s="2"/>
+      <c r="F141" s="5"/>
       <c r="G141" s="2"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>444</v>
       </c>
@@ -4589,10 +4604,10 @@
       <c r="E142" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F142" s="2"/>
+      <c r="F142" s="5"/>
       <c r="G142" s="2"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>447</v>
       </c>
@@ -4608,10 +4623,10 @@
       <c r="E143" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F143" s="2"/>
+      <c r="F143" s="5"/>
       <c r="G143" s="2"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>450</v>
       </c>
@@ -4627,10 +4642,10 @@
       <c r="E144" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F144" s="2"/>
+      <c r="F144" s="5"/>
       <c r="G144" s="2"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>453</v>
       </c>
@@ -4646,10 +4661,10 @@
       <c r="E145" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F145" s="2"/>
+      <c r="F145" s="5"/>
       <c r="G145" s="2"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>456</v>
       </c>
@@ -4665,10 +4680,10 @@
       <c r="E146" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F146" s="2"/>
+      <c r="F146" s="5"/>
       <c r="G146" s="2"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>459</v>
       </c>
@@ -4684,10 +4699,10 @@
       <c r="E147" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F147" s="2"/>
+      <c r="F147" s="5"/>
       <c r="G147" s="2"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>462</v>
       </c>
@@ -4703,10 +4718,10 @@
       <c r="E148" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F148" s="2"/>
+      <c r="F148" s="5"/>
       <c r="G148" s="2"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>465</v>
       </c>
@@ -4722,10 +4737,10 @@
       <c r="E149" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="F149" s="2"/>
+      <c r="F149" s="5"/>
       <c r="G149" s="2"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>468</v>
       </c>
@@ -4741,10 +4756,10 @@
       <c r="E150" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F150" s="2"/>
+      <c r="F150" s="5"/>
       <c r="G150" s="2"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
         <v>472</v>
       </c>
@@ -4760,10 +4775,10 @@
       <c r="E151" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="F151" s="2"/>
+      <c r="F151" s="5"/>
       <c r="G151" s="2"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>475</v>
       </c>
@@ -4779,10 +4794,10 @@
       <c r="E152" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F152" s="2"/>
+      <c r="F152" s="5"/>
       <c r="G152" s="2"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>478</v>
       </c>
@@ -4798,10 +4813,10 @@
       <c r="E153" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F153" s="2"/>
+      <c r="F153" s="5"/>
       <c r="G153" s="2"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>481</v>
       </c>
@@ -4817,11 +4832,19 @@
       <c r="E154" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F154" s="2"/>
+      <c r="F154" s="5"/>
       <c r="G154" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E154" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E154" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="IT_Team_3"/>
+        <filter val="IT_Team_4"/>
+        <filter val="IT_Team_5"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>